<commit_message>
Clean and submit PA2
</commit_message>
<xml_diff>
--- a/Doc/TaskProgresReport.xlsx
+++ b/Doc/TaskProgresReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -77,6 +77,36 @@
   </si>
   <si>
     <t xml:space="preserve">Wrote pseudo for main.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created Config.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created Individuals.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set up dictionary for configs in Individuals.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked on csv import methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked on dataframe objects in Individuals.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked on line graphs in Individuals.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked on query functionality in Individuals.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked on violin plots in Individuals.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleaned up Individuals.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tested method functionality of Individuals.py</t>
   </si>
 </sst>
 </file>
@@ -297,10 +327,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -479,6 +509,146 @@
         <v>8</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="n">
+        <v>45610</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
+        <v>45610</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="n">
+        <v>45615</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="n">
+        <v>45615</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="n">
+        <v>45615</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="n">
+        <v>45615</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="n">
+        <v>45616</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="n">
+        <v>45616</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="n">
+        <v>45616</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="n">
+        <v>45616</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>